<commit_message>
Remove blocking auto-calculations from van der Werf.xlsx
</commit_message>
<xml_diff>
--- a/Excel/van der Werf.xlsx
+++ b/Excel/van der Werf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cclea\source\repos\beefblup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7872F19D-AED9-4EFB-A292-767BDE335357}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC97A62B-8BB9-4BA6-A72C-1957A7453EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="12648" xr2:uid="{F6178493-5AB1-4A33-B063-77A473B245B4}"/>
+    <workbookView xWindow="4164" yWindow="960" windowWidth="17280" windowHeight="9108" xr2:uid="{F6178493-5AB1-4A33-B063-77A473B245B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Animal ID</t>
   </si>
@@ -45,9 +47,6 @@
     <t>Birth Date</t>
   </si>
   <si>
-    <t>Age of Dam</t>
-  </si>
-  <si>
     <t>Sex</t>
   </si>
   <si>
@@ -63,31 +62,10 @@
     <t>Birth Weight</t>
   </si>
   <si>
-    <t>Herd</t>
-  </si>
-  <si>
-    <t>Season</t>
-  </si>
-  <si>
-    <t>Breed</t>
-  </si>
-  <si>
-    <t>ET?</t>
-  </si>
-  <si>
     <t>Age of Dam (Days - Hidden)</t>
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>van der Werf</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>FALSE</t>
   </si>
   <si>
     <t>2</t>
@@ -226,22 +204,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -251,9 +223,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -280,7 +249,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
@@ -768,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98A6E87-8A4D-4AF0-822B-ACEFAAC4D94B}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,342 +748,208 @@
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>32874</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13">
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10">
         <v>354</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2:F65" si="0">IFERROR(_xlfn.DAYS(B2,VLOOKUP(C2,$A$2:$M$220,2,FALSE)),"")</f>
+        <f>IFERROR(_xlfn.DAYS(B2,VLOOKUP(C2,$A$2:$H$220,2,FALSE)),"")</f>
         <v/>
       </c>
-      <c r="G2" s="11">
-        <f t="shared" ref="G2:G65" si="1">YEAR(B2)</f>
+      <c r="G2" s="8">
+        <f t="shared" ref="G2:G8" si="0">YEAR(B2)</f>
         <v>1990</v>
       </c>
-      <c r="H2" s="11" t="str">
-        <f>IF(MONTH(B2)&lt;7,"Spring","Fall")</f>
-        <v>Spring</v>
-      </c>
-      <c r="I2" s="12" t="str">
-        <f t="shared" ref="I2:I65" si="2">IF(F2&lt;1004,2,IF(F2&lt;1369,3,IF(F2&lt;1734,4,IF(F2&lt;3560,5,IF(F2&lt;3925,10,IF(F2&lt;4291,11,IF(F2&lt;4656,12,IF(F2="","",13))))))))</f>
-        <v/>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>18</v>
+      <c r="H2" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>19</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>32874</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13">
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10">
         <v>251</v>
       </c>
       <c r="F3" t="str">
+        <f>IFERROR(_xlfn.DAYS(B3,VLOOKUP(C3,$A$2:$H$220,2,FALSE)),"")</f>
+        <v/>
+      </c>
+      <c r="G3" s="8">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G3" s="11">
-        <f t="shared" si="1"/>
         <v>1990</v>
       </c>
-      <c r="H3" s="11" t="str">
-        <f t="shared" ref="H3:H66" si="3">IF(MONTH(B3)&lt;7,"Spring","Fall")</f>
-        <v>Spring</v>
-      </c>
-      <c r="I3" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>18</v>
+      <c r="H3" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>20</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="B4" s="1">
         <v>33239</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="13">
+      <c r="C4" s="8"/>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="10">
         <v>327</v>
       </c>
       <c r="F4" t="str">
+        <f>IFERROR(_xlfn.DAYS(B4,VLOOKUP(C4,$A$2:$H$220,2,FALSE)),"")</f>
+        <v/>
+      </c>
+      <c r="G4" s="8">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G4" s="11">
-        <f t="shared" si="1"/>
         <v>1991</v>
       </c>
-      <c r="H4" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>Spring</v>
-      </c>
-      <c r="I4" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>18</v>
+      <c r="H4" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>21</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>33239</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="13">
+      <c r="C5" s="8"/>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10">
         <v>328</v>
       </c>
       <c r="F5" t="str">
+        <f>IFERROR(_xlfn.DAYS(B5,VLOOKUP(C5,$A$2:$H$220,2,FALSE)),"")</f>
+        <v/>
+      </c>
+      <c r="G5" s="8">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="1"/>
         <v>1991</v>
       </c>
-      <c r="H5" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>Spring</v>
-      </c>
-      <c r="I5" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>18</v>
+      <c r="H5" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>22</v>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>33239</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="10">
+        <v>301</v>
+      </c>
+      <c r="F6">
+        <f>IFERROR(_xlfn.DAYS(B6,VLOOKUP(C6,$A$2:$H$220,2,FALSE)),"")</f>
+        <v>365</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="0"/>
+        <v>1991</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="E6" s="13">
-        <v>301</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>365</v>
-      </c>
-      <c r="G6" s="11">
-        <f t="shared" si="1"/>
-        <v>1991</v>
-      </c>
-      <c r="H6" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>Spring</v>
-      </c>
-      <c r="I6" s="12">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="B7" s="1">
         <v>33239</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13">
+      <c r="C7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10">
         <v>270</v>
       </c>
       <c r="F7">
+        <f>IFERROR(_xlfn.DAYS(B7,VLOOKUP(C7,$A$2:$H$220,2,FALSE)),"")</f>
+        <v>365</v>
+      </c>
+      <c r="G7" s="8">
         <f t="shared" si="0"/>
-        <v>365</v>
-      </c>
-      <c r="G7" s="11">
-        <f t="shared" si="1"/>
         <v>1991</v>
       </c>
-      <c r="H7" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>Spring</v>
-      </c>
-      <c r="I7" s="12">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J7" s="11" t="s">
+      <c r="H7" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="B8" s="1">
         <v>33604</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13">
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10">
         <v>330</v>
       </c>
       <c r="F8" t="str">
+        <f>IFERROR(_xlfn.DAYS(B8,VLOOKUP(C8,$A$2:$H$220,2,FALSE)),"")</f>
+        <v/>
+      </c>
+      <c r="G8" s="8">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G8" s="11">
-        <f t="shared" si="1"/>
         <v>1992</v>
       </c>
-      <c r="H8" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>Spring</v>
-      </c>
-      <c r="I8" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>18</v>
+      <c r="H8" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed instructions from van der Werf example
</commit_message>
<xml_diff>
--- a/Excel/van der Werf.xlsx
+++ b/Excel/van der Werf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cclea\source\repos\beefblup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC97A62B-8BB9-4BA6-A72C-1957A7453EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466CFD27-A69D-4010-9595-6F00FA1D8E01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4164" yWindow="960" windowWidth="17280" windowHeight="9108" xr2:uid="{F6178493-5AB1-4A33-B063-77A473B245B4}"/>
+    <workbookView xWindow="-48" yWindow="324" windowWidth="23136" windowHeight="12360" xr2:uid="{F6178493-5AB1-4A33-B063-77A473B245B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -243,201 +243,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="4096827" cy="3238500"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8060B58A-69A1-4238-BB71-D953EB73DDE9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9608820" y="937260"/>
-          <a:ext cx="4096827" cy="3238500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Master BLUP</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> Worksheet by Thomas A. Christensen II</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>https://github.com/millironx/beefblup</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>To use: fill in the table with your herd's data underneath the </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>GREEN</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>, </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>YELLOW</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>, and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>PURPLE</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> headers</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>GREEN</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>: Basic ID and pedigree information</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>BLUE</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>: Year, Season and Age-Of-Dam contemporary grouping information automatically calculuated from the info in the GREEN section. DO NOT modify these formulas!</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>YELLOW</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>: Observed trait</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>PURPLE</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>: Additional contemporary grouping information that cannot be surmised from other parts of the data</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>The contemporary groupings given in this sheet reflect current (2018) Beef Improvement Federation guidelines for comparing birth weight data. Appropriate columns should be added or removed from the </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>PURPLE</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> section to evaluate other traits.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -787,11 +592,11 @@
         <v>354</v>
       </c>
       <c r="F2" t="str">
-        <f>IFERROR(_xlfn.DAYS(B2,VLOOKUP(C2,$A$2:$H$220,2,FALSE)),"")</f>
+        <f t="shared" ref="F2:F8" si="0">IFERROR(_xlfn.DAYS(B2,VLOOKUP(C2,$A$2:$H$220,2,FALSE)),"")</f>
         <v/>
       </c>
       <c r="G2" s="8">
-        <f t="shared" ref="G2:G8" si="0">YEAR(B2)</f>
+        <f t="shared" ref="G2:G8" si="1">YEAR(B2)</f>
         <v>1990</v>
       </c>
       <c r="H2" s="8" t="s">
@@ -811,11 +616,11 @@
         <v>251</v>
       </c>
       <c r="F3" t="str">
-        <f>IFERROR(_xlfn.DAYS(B3,VLOOKUP(C3,$A$2:$H$220,2,FALSE)),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G3" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1990</v>
       </c>
       <c r="H3" s="8" t="s">
@@ -837,11 +642,11 @@
         <v>327</v>
       </c>
       <c r="F4" t="str">
-        <f>IFERROR(_xlfn.DAYS(B4,VLOOKUP(C4,$A$2:$H$220,2,FALSE)),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1991</v>
       </c>
       <c r="H4" s="8" t="s">
@@ -863,11 +668,11 @@
         <v>328</v>
       </c>
       <c r="F5" t="str">
-        <f>IFERROR(_xlfn.DAYS(B5,VLOOKUP(C5,$A$2:$H$220,2,FALSE)),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1991</v>
       </c>
       <c r="H5" s="8" t="s">
@@ -891,11 +696,11 @@
         <v>301</v>
       </c>
       <c r="F6">
-        <f>IFERROR(_xlfn.DAYS(B6,VLOOKUP(C6,$A$2:$H$220,2,FALSE)),"")</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="G6" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1991</v>
       </c>
       <c r="H6" s="8" t="s">
@@ -917,11 +722,11 @@
         <v>270</v>
       </c>
       <c r="F7">
-        <f>IFERROR(_xlfn.DAYS(B7,VLOOKUP(C7,$A$2:$H$220,2,FALSE)),"")</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="G7" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1991</v>
       </c>
       <c r="H7" s="8" t="s">
@@ -941,11 +746,11 @@
         <v>330</v>
       </c>
       <c r="F8" t="str">
-        <f>IFERROR(_xlfn.DAYS(B8,VLOOKUP(C8,$A$2:$H$220,2,FALSE)),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G8" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1992</v>
       </c>
       <c r="H8" s="8" t="s">
@@ -954,6 +759,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>